<commit_message>
I wrote a sumif
</commit_message>
<xml_diff>
--- a/第2章 初识Excel函数/2.1.2 培养应用函数的意识.xlsx
+++ b/第2章 初识Excel函数/2.1.2 培养应用函数的意识.xlsx
@@ -927,16 +927,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -956,10 +956,78 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -969,14 +1037,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1261,7 +1329,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2743,6 +2811,10 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B58">
+        <f>SUMIF(E$44:E$56,2,F$44:F$56)</f>
+        <v>11</v>
+      </c>
       <c r="H58" s="11">
         <f>SUMPRODUCT(E2:E56,F2:F56)</f>
         <v>80</v>

</xml_diff>